<commit_message>
fixed an error with the hoverCam modes
</commit_message>
<xml_diff>
--- a/ResearchDiary/Questionnaires/TrackedData.xlsx
+++ b/ResearchDiary/Questionnaires/TrackedData.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmaer\Documents\FH\Projects\MasterArbeit\mmt-masterarbeit-david-maerzendorfer\ResearchDiary\Questionnaires\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C842F81-145F-4082-A4D1-0BAB07012E51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4301C5E-23E2-4C21-9B7B-789487C74761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Demo" sheetId="1" r:id="rId1"/>
+    <sheet name="RealData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="59">
   <si>
     <t>Mode</t>
   </si>
@@ -172,6 +173,36 @@
   </si>
   <si>
     <t>eva</t>
+  </si>
+  <si>
+    <t>above are old ones</t>
+  </si>
+  <si>
+    <t>PoiNameOne</t>
+  </si>
+  <si>
+    <t>PoiNameTwo</t>
+  </si>
+  <si>
+    <t>PoiNameThree</t>
+  </si>
+  <si>
+    <t>PoiNameFour</t>
+  </si>
+  <si>
+    <t>PoiNameFive</t>
+  </si>
+  <si>
+    <t>PoiNameSix</t>
+  </si>
+  <si>
+    <t>Dodo</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>16.10.24</t>
   </si>
 </sst>
 </file>
@@ -207,13 +238,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="20">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -224,7 +263,112 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -518,11 +662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V5"/>
+  <dimension ref="A1:V8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V5" sqref="V5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -827,24 +970,321 @@
         <v>47</v>
       </c>
     </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:XFD4 A6:XFD32 A5">
-    <cfRule type="expression" dxfId="3" priority="1">
+  <conditionalFormatting sqref="A8:XFD32 A2:XFD4 A5 A6:XFD6 A7:C7">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>$B2="Drone"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="4" priority="3">
       <formula>$B2="Hover"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:XFD5">
-    <cfRule type="expression" dxfId="1" priority="5">
+    <cfRule type="expression" dxfId="3" priority="6">
       <formula>$C5="Drone"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="6">
+    <cfRule type="expression" dxfId="2" priority="7">
       <formula>$C5="Hover"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBBC2517-9B67-445D-A041-4C30D5ABB61A}">
+  <dimension ref="A1:AB45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="7.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="22.08984375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="23.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" t="s">
+        <v>53</v>
+      </c>
+      <c r="P1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>11</v>
+      </c>
+      <c r="R1" t="s">
+        <v>54</v>
+      </c>
+      <c r="S1" t="s">
+        <v>12</v>
+      </c>
+      <c r="T1" t="s">
+        <v>13</v>
+      </c>
+      <c r="U1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V1" t="s">
+        <v>14</v>
+      </c>
+      <c r="W1" t="s">
+        <v>15</v>
+      </c>
+      <c r="X1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B27" s="1"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B28" s="1"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B30" s="1"/>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B33" s="1"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B34" s="1"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B35" s="1"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B36" s="1"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B37" s="1"/>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B38" s="1"/>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B39" s="1"/>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B40" s="1"/>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B41" s="1"/>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B42" s="1"/>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B43" s="1"/>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B44" s="1"/>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B45" s="1"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A2:XFD62">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>$C2="Hover"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>$C2="Drone"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>